<commit_message>
- nexial filter now supported in flow control as well as CSV Expression (already the case since 1.0) - added more conditions to nexial filter. Now the complete list is:  - >, >=, <, <=, =, !=, is/in, is not/not in, contain, start with, end with, is undefined, is defined, has length of, is empty, is not empty, match (regex) - nexial filter now uses pipe (`|`) as separate for item listing.  item listing should be enclosed in [...] unless there's only 1 item.
[CSV expression]
- `removeColumns` now supports one or many columns referenced by name or index (zero-based)

Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/image-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/image-showcase.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23863" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24703" uniqueCount="456">
   <si>
     <t>jira</t>
   </si>
@@ -1417,6 +1417,15 @@
   </si>
   <si>
     <t>storeKeys(var,profile,keyPattern)</t>
+  </si>
+  <si>
+    <t>saveRowCount(var)</t>
+  </si>
+  <si>
+    <t>saveTableRowsRange(var,beginRow,endRow)</t>
+  </si>
+  <si>
+    <t>assertBetween(num,min,max)</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1433,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="732" x14ac:knownFonts="1">
+  <fonts count="756" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6067,8 +6076,160 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1264">
+  <fills count="1306">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13227,8 +13388,246 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1203">
+  <borders count="1243">
     <border>
       <left/>
       <right/>
@@ -13265,6 +13664,394 @@
         <color theme="2" tint="-0.749961851863155"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -24913,7 +25700,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="757">
+  <cellXfs count="781">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -27166,40 +27953,112 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="719" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="720" fillId="1245" borderId="1190" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="721" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1190" fillId="1245" fontId="720" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="721" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="722" fillId="1248" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1248" fontId="722" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="723" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="724" fillId="1251" borderId="1194" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="725" fillId="1254" borderId="1198" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="726" fillId="1257" borderId="1202" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="727" fillId="1257" borderId="1202" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="728" fillId="1260" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="729" fillId="1263" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="730" fillId="1260" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="731" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="723" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1194" fillId="1251" fontId="724" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1198" fillId="1254" fontId="725" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1202" fillId="1257" fontId="726" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1202" fillId="1257" fontId="727" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1260" fontId="728" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1263" fontId="729" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1260" fontId="730" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="731" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1210" fillId="1266" fontId="732" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="733" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1269" fontId="734" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="735" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1214" fillId="1272" fontId="736" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1218" fillId="1275" fontId="737" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1222" fillId="1278" fontId="738" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1222" fillId="1278" fontId="739" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1281" fontId="740" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1284" fontId="741" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1281" fontId="742" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="743" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="744" fillId="1287" borderId="1230" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="745" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="746" fillId="1290" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="747" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="748" fillId="1293" borderId="1234" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="749" fillId="1296" borderId="1238" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="750" fillId="1299" borderId="1242" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="751" fillId="1299" borderId="1242" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="752" fillId="1302" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="753" fillId="1305" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="754" fillId="1302" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="755" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -27641,7 +28500,7 @@
         <v>202</v>
       </c>
       <c r="M2" t="s">
-        <v>435</v>
+        <v>455</v>
       </c>
       <c r="N2" t="s">
         <v>259</v>
@@ -28605,7 +29464,7 @@
     </row>
     <row r="52">
       <c r="E52" t="s">
-        <v>394</v>
+        <v>343</v>
       </c>
       <c r="S52" t="s">
         <v>136</v>
@@ -28613,7 +29472,7 @@
     </row>
     <row r="53">
       <c r="E53" t="s">
-        <v>395</v>
+        <v>274</v>
       </c>
       <c r="S53" t="s">
         <v>137</v>
@@ -28621,7 +29480,7 @@
     </row>
     <row r="54">
       <c r="E54" t="s">
-        <v>343</v>
+        <v>298</v>
       </c>
       <c r="S54" t="s">
         <v>138</v>
@@ -28629,7 +29488,7 @@
     </row>
     <row r="55">
       <c r="E55" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="S55" t="s">
         <v>139</v>
@@ -28637,7 +29496,7 @@
     </row>
     <row r="56">
       <c r="E56" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="S56" t="s">
         <v>140</v>
@@ -28645,7 +29504,7 @@
     </row>
     <row r="57">
       <c r="E57" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="S57" t="s">
         <v>141</v>
@@ -28653,7 +29512,7 @@
     </row>
     <row r="58">
       <c r="E58" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="S58" t="s">
         <v>220</v>
@@ -28661,7 +29520,7 @@
     </row>
     <row r="59">
       <c r="E59" t="s">
-        <v>310</v>
+        <v>350</v>
       </c>
       <c r="S59" t="s">
         <v>430</v>
@@ -28669,7 +29528,7 @@
     </row>
     <row r="60">
       <c r="E60" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="S60" t="s">
         <v>142</v>
@@ -28677,7 +29536,7 @@
     </row>
     <row r="61">
       <c r="E61" t="s">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="S61" t="s">
         <v>143</v>
@@ -28685,7 +29544,7 @@
     </row>
     <row r="62">
       <c r="E62" t="s">
-        <v>317</v>
+        <v>410</v>
       </c>
       <c r="S62" t="s">
         <v>144</v>
@@ -28693,7 +29552,7 @@
     </row>
     <row r="63">
       <c r="E63" t="s">
-        <v>318</v>
+        <v>411</v>
       </c>
       <c r="S63" t="s">
         <v>145</v>
@@ -28701,7 +29560,7 @@
     </row>
     <row r="64">
       <c r="E64" t="s">
-        <v>410</v>
+        <v>358</v>
       </c>
       <c r="S64" t="s">
         <v>203</v>
@@ -28709,7 +29568,7 @@
     </row>
     <row r="65">
       <c r="E65" t="s">
-        <v>411</v>
+        <v>321</v>
       </c>
       <c r="S65" t="s">
         <v>204</v>
@@ -28717,7 +29576,7 @@
     </row>
     <row r="66">
       <c r="E66" t="s">
-        <v>358</v>
+        <v>275</v>
       </c>
       <c r="S66" t="s">
         <v>146</v>
@@ -28725,7 +29584,7 @@
     </row>
     <row r="67">
       <c r="E67" t="s">
-        <v>321</v>
+        <v>390</v>
       </c>
       <c r="S67" t="s">
         <v>147</v>
@@ -28733,7 +29592,7 @@
     </row>
     <row r="68">
       <c r="E68" t="s">
-        <v>275</v>
+        <v>322</v>
       </c>
       <c r="S68" t="s">
         <v>148</v>
@@ -28741,7 +29600,7 @@
     </row>
     <row r="69">
       <c r="E69" t="s">
-        <v>390</v>
+        <v>453</v>
       </c>
       <c r="S69" t="s">
         <v>149</v>
@@ -28749,7 +29608,7 @@
     </row>
     <row r="70">
       <c r="E70" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="S70" t="s">
         <v>150</v>
@@ -28757,7 +29616,7 @@
     </row>
     <row r="71">
       <c r="E71" t="s">
-        <v>312</v>
+        <v>454</v>
       </c>
       <c r="S71" t="s">
         <v>205</v>

</xml_diff>